<commit_message>
Main creation and loa fixing
The new main calls the functions:
add_education_indicators
run_education_analysis
change_label
create_access_education_table
create_out_of_school_education_table
create_ece_table
create_level_education_table

Update the edu_helper_table and fix the loa for incoherence between levels.

still problems with barrier labeling
</commit_message>
<xml_diff>
--- a/input_tool/edu_indicator_labelling.xlsx
+++ b/input_tool/edu_indicator_labelling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/MSNAEdu/EduAnalysisTool/input_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{D3462D9F-D80F-4473-B948-1519E83722D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40D14ADA-1DCA-4E85-A672-F4D60769437E}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{D3462D9F-D80F-4473-B948-1519E83722D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{190ED58C-445D-4F04-8913-6287FBB6F071}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15990" yWindow="-18120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="update_survey" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="381">
   <si>
     <t>theme</t>
   </si>
@@ -1027,15 +1027,9 @@
     <t>Phase 5 FCLC</t>
   </si>
   <si>
-    <t>% of children (one year before the official primary school entry age) who are attending an early childhood education programme or primary school</t>
-  </si>
-  <si>
     <t>edu_attending_level0_level1_and_level1_minus_one_age_d</t>
   </si>
   <si>
-    <t>% of children in the relevant age group (one year before the official primary school entry age) who are attending primary school</t>
-  </si>
-  <si>
     <t>edu_attending_level1_and_level1_minus_one_age_d</t>
   </si>
   <si>
@@ -1147,15 +1141,9 @@
     <t>Nombre d'individus en âge de scolarisation</t>
   </si>
   <si>
-    <t>% d'enfants (un an avant l'âge d'entrée à l'école primaire) en programme pré-primaire ou primaire</t>
-  </si>
-  <si>
     <t>% of school-aged children  who did not attend school or any early childhood education program at any time during the 2023-2024 school year</t>
   </si>
   <si>
-    <t>% d'enfants (un an avant l'âge d'entrée à l'école primaire) en primaire</t>
-  </si>
-  <si>
     <t>% d'enfants en âge de fréquenter l'école primaire ou plus</t>
   </si>
   <si>
@@ -1165,9 +1153,6 @@
     <t>% d'enfants en âge de secondaire actuellement scolarisés au secondaire ou plus</t>
   </si>
   <si>
-    <t>% d'enfants en âge de primaire actuellement scolarisés au primaire ou plus</t>
-  </si>
-  <si>
     <t>% d'enfants en âge de niveau intermédiaire actuellement scolarisés au niveau intermédiaire ou plus</t>
   </si>
   <si>
@@ -1190,6 +1175,18 @@
   </si>
   <si>
     <t>1. % de ménages avec enfants de 5 à 18 ans par moyens d'améliorer l'éducation</t>
+  </si>
+  <si>
+    <t>% of children one year before primary school entry age attending early childhood education or primary school.</t>
+  </si>
+  <si>
+    <t>% of children one year before primary school entry age attending primary school.</t>
+  </si>
+  <si>
+    <t>% d'enfants un an avant l'âge d'entrée à l'école primaire fréquentant un programme d'éducation préscolaire ou l'école primaire</t>
+  </si>
+  <si>
+    <t>% d'enfants un an avant l'âge d'entrée à l'école primaire fréquentant l'école primaire</t>
   </si>
 </sst>
 </file>
@@ -1611,22 +1608,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.75" x14ac:dyDescent="0.95"/>
   <cols>
     <col min="1" max="1" width="13.75" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="41.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="94.875" style="4" customWidth="1"/>
     <col min="5" max="5" width="52.25" style="4" customWidth="1"/>
     <col min="6" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.95">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1643,7 +1640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.95">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1654,13 +1651,13 @@
         <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.95">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1671,13 +1668,13 @@
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E3" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.95">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1688,13 +1685,13 @@
         <v>10</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E4" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.95">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1705,13 +1702,13 @@
         <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E5" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.95">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1722,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.95">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1739,13 +1736,13 @@
         <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E7" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.95">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1759,10 +1756,10 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.95">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1776,10 +1773,10 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1787,16 +1784,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="D10" s="8" t="s">
         <v>327</v>
       </c>
+      <c r="D10" t="s">
+        <v>377</v>
+      </c>
       <c r="E10" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1804,16 +1801,16 @@
         <v>7</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>329</v>
+        <v>378</v>
       </c>
       <c r="E11" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -1821,16 +1818,16 @@
         <v>7</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E12" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1838,16 +1835,16 @@
         <v>7</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E13" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1855,16 +1852,16 @@
         <v>7</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E14" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1872,16 +1869,16 @@
         <v>7</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E15" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1889,16 +1886,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E16" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1906,16 +1903,16 @@
         <v>7</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E17" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -1923,16 +1920,16 @@
         <v>7</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E18" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -1940,16 +1937,16 @@
         <v>7</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E19" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -1957,16 +1954,16 @@
         <v>7</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E20" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -1974,16 +1971,16 @@
         <v>7</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E21" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="25.5" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="26.5" x14ac:dyDescent="0.95">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -1991,16 +1988,16 @@
         <v>7</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E22" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="38.25" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="39.75" x14ac:dyDescent="0.95">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
@@ -2008,16 +2005,16 @@
         <v>7</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E23" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.95">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -2025,24 +2022,24 @@
         <v>7</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.95">
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.95">
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.95">
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
@@ -2066,7 +2063,7 @@
       <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.75" x14ac:dyDescent="0.95"/>
   <cols>
     <col min="1" max="1" width="36.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="21.5" style="6" customWidth="1"/>
@@ -2076,7 +2073,7 @@
     <col min="9" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -2102,7 +2099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -2116,7 +2113,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
@@ -2130,7 +2127,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -2144,7 +2141,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -2158,7 +2155,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
@@ -2172,7 +2169,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
@@ -2186,7 +2183,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -2200,7 +2197,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A10" s="6" t="s">
         <v>35</v>
       </c>
@@ -2214,7 +2211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A11" s="6" t="s">
         <v>35</v>
       </c>
@@ -2228,7 +2225,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -2242,7 +2239,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A14" s="6" t="s">
         <v>53</v>
       </c>
@@ -2256,7 +2253,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A15" s="6" t="s">
         <v>53</v>
       </c>
@@ -2270,7 +2267,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.95">
       <c r="A16" s="6" t="s">
         <v>53</v>
       </c>
@@ -2284,7 +2281,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A17" s="6" t="s">
         <v>53</v>
       </c>
@@ -2298,7 +2295,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A18" s="6" t="s">
         <v>53</v>
       </c>
@@ -2312,7 +2309,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A20" s="6" t="s">
         <v>66</v>
       </c>
@@ -2326,7 +2323,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A21" s="6" t="s">
         <v>66</v>
       </c>
@@ -2340,7 +2337,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A22" s="6" t="s">
         <v>66</v>
       </c>
@@ -2354,7 +2351,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A23" s="6" t="s">
         <v>66</v>
       </c>
@@ -2368,7 +2365,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A24" s="6" t="s">
         <v>66</v>
       </c>
@@ -2382,7 +2379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A25" s="6" t="s">
         <v>66</v>
       </c>
@@ -2396,7 +2393,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A26" s="6" t="s">
         <v>66</v>
       </c>
@@ -2410,7 +2407,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A27" s="6" t="s">
         <v>66</v>
       </c>
@@ -2424,7 +2421,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A28" s="6" t="s">
         <v>66</v>
       </c>
@@ -2438,7 +2435,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A29" s="6" t="s">
         <v>66</v>
       </c>
@@ -2452,7 +2449,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A31" s="6" t="s">
         <v>83</v>
       </c>
@@ -2466,7 +2463,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A32" s="6" t="s">
         <v>83</v>
       </c>
@@ -2480,7 +2477,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A33" s="6" t="s">
         <v>83</v>
       </c>
@@ -2494,7 +2491,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A34" s="6" t="s">
         <v>83</v>
       </c>
@@ -2508,7 +2505,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A36" s="6" t="s">
         <v>92</v>
       </c>
@@ -2522,7 +2519,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A37" s="6" t="s">
         <v>92</v>
       </c>
@@ -2536,7 +2533,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A38" s="6" t="s">
         <v>92</v>
       </c>
@@ -2550,7 +2547,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A39" s="6" t="s">
         <v>92</v>
       </c>
@@ -2564,7 +2561,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A41" s="6" t="s">
         <v>103</v>
       </c>
@@ -2578,7 +2575,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A42" s="6" t="s">
         <v>103</v>
       </c>
@@ -2592,7 +2589,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A43" s="6" t="s">
         <v>103</v>
       </c>
@@ -2606,7 +2603,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A45" s="6" t="s">
         <v>113</v>
       </c>
@@ -2620,7 +2617,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A46" s="6" t="s">
         <v>113</v>
       </c>
@@ -2634,7 +2631,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A47" s="6" t="s">
         <v>113</v>
       </c>
@@ -2648,7 +2645,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A48" s="6" t="s">
         <v>113</v>
       </c>
@@ -2662,7 +2659,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A50" s="6" t="s">
         <v>123</v>
       </c>
@@ -2676,7 +2673,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A51" s="6" t="s">
         <v>123</v>
       </c>
@@ -2690,7 +2687,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A52" s="6" t="s">
         <v>123</v>
       </c>
@@ -2704,7 +2701,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A53" s="6" t="s">
         <v>123</v>
       </c>
@@ -2718,7 +2715,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A55" s="6" t="s">
         <v>130</v>
       </c>
@@ -2732,7 +2729,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A56" s="6" t="s">
         <v>130</v>
       </c>
@@ -2746,7 +2743,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A57" s="6" t="s">
         <v>130</v>
       </c>
@@ -2760,7 +2757,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A58" s="6" t="s">
         <v>130</v>
       </c>
@@ -2774,7 +2771,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A59" s="6" t="s">
         <v>130</v>
       </c>
@@ -2788,7 +2785,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A61" s="1" t="s">
         <v>140</v>
       </c>
@@ -2802,7 +2799,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A62" s="1" t="s">
         <v>140</v>
       </c>
@@ -2816,7 +2813,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A63" s="1" t="s">
         <v>140</v>
       </c>
@@ -2830,7 +2827,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A64" s="1" t="s">
         <v>140</v>
       </c>
@@ -2844,7 +2841,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A66" s="6" t="s">
         <v>144</v>
       </c>
@@ -2858,7 +2855,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A67" s="6" t="s">
         <v>144</v>
       </c>
@@ -2872,7 +2869,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A68" s="6" t="s">
         <v>144</v>
       </c>
@@ -2886,7 +2883,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A69" s="6" t="s">
         <v>144</v>
       </c>
@@ -2900,7 +2897,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A71" s="6" t="s">
         <v>155</v>
       </c>
@@ -2914,7 +2911,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A72" s="6" t="s">
         <v>155</v>
       </c>
@@ -2928,7 +2925,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A73" s="6" t="s">
         <v>155</v>
       </c>
@@ -2942,7 +2939,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A74" s="6" t="s">
         <v>155</v>
       </c>
@@ -2956,7 +2953,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A76" s="6" t="s">
         <v>165</v>
       </c>
@@ -2970,7 +2967,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A77" s="6" t="s">
         <v>165</v>
       </c>
@@ -2984,7 +2981,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A78" s="6" t="s">
         <v>165</v>
       </c>
@@ -2998,7 +2995,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A79" s="6" t="s">
         <v>165</v>
       </c>
@@ -3012,7 +3009,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A80" s="6" t="s">
         <v>165</v>
       </c>
@@ -3026,7 +3023,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A82" s="6" t="s">
         <v>174</v>
       </c>
@@ -3040,7 +3037,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A83" s="6" t="s">
         <v>174</v>
       </c>
@@ -3054,7 +3051,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A84" s="6" t="s">
         <v>174</v>
       </c>
@@ -3068,7 +3065,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A85" s="6" t="s">
         <v>174</v>
       </c>
@@ -3082,7 +3079,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A87" s="6" t="s">
         <v>179</v>
       </c>
@@ -3096,7 +3093,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A88" s="6" t="s">
         <v>179</v>
       </c>
@@ -3110,7 +3107,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A89" s="6" t="s">
         <v>179</v>
       </c>
@@ -3124,7 +3121,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A90" s="6" t="s">
         <v>179</v>
       </c>
@@ -3138,7 +3135,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A91" s="6" t="s">
         <v>179</v>
       </c>
@@ -3152,7 +3149,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A92" s="6" t="s">
         <v>179</v>
       </c>
@@ -3166,7 +3163,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A93" s="6" t="s">
         <v>179</v>
       </c>
@@ -3180,7 +3177,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A94" s="6" t="s">
         <v>179</v>
       </c>
@@ -3194,7 +3191,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A95" s="6" t="s">
         <v>179</v>
       </c>
@@ -3208,7 +3205,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A96" s="6" t="s">
         <v>179</v>
       </c>
@@ -3222,7 +3219,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A97" s="6" t="s">
         <v>179</v>
       </c>
@@ -3236,7 +3233,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A98" s="6" t="s">
         <v>179</v>
       </c>
@@ -3250,7 +3247,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A99" s="6" t="s">
         <v>179</v>
       </c>
@@ -3264,7 +3261,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A100" s="6" t="s">
         <v>179</v>
       </c>
@@ -3278,7 +3275,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A101" s="6" t="s">
         <v>179</v>
       </c>
@@ -3292,7 +3289,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A102" s="6" t="s">
         <v>179</v>
       </c>
@@ -3306,7 +3303,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A103" s="6" t="s">
         <v>179</v>
       </c>
@@ -3320,7 +3317,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A104" s="6" t="s">
         <v>179</v>
       </c>
@@ -3334,7 +3331,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A105" s="6" t="s">
         <v>179</v>
       </c>
@@ -3348,7 +3345,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A106" s="6" t="s">
         <v>179</v>
       </c>
@@ -3362,7 +3359,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A107" s="6" t="s">
         <v>179</v>
       </c>
@@ -3376,7 +3373,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A108" s="6" t="s">
         <v>179</v>
       </c>
@@ -3390,7 +3387,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A109" s="6" t="s">
         <v>179</v>
       </c>
@@ -3404,7 +3401,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A110" s="6" t="s">
         <v>179</v>
       </c>
@@ -3418,7 +3415,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A112" s="6" t="s">
         <v>228</v>
       </c>
@@ -3432,7 +3429,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A113" s="6" t="s">
         <v>228</v>
       </c>
@@ -3446,7 +3443,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A115" s="6" t="s">
         <v>235</v>
       </c>
@@ -3460,7 +3457,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A116" s="6" t="s">
         <v>235</v>
       </c>
@@ -3474,7 +3471,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A118" s="6" t="s">
         <v>236</v>
       </c>
@@ -3488,7 +3485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A119" s="6" t="s">
         <v>236</v>
       </c>
@@ -3502,7 +3499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A121" s="6" t="s">
         <v>237</v>
       </c>
@@ -3516,7 +3513,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A122" s="6" t="s">
         <v>237</v>
       </c>
@@ -3530,7 +3527,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A123" s="6" t="s">
         <v>237</v>
       </c>
@@ -3544,7 +3541,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A125" s="6" t="s">
         <v>247</v>
       </c>
@@ -3558,7 +3555,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A126" s="6" t="s">
         <v>247</v>
       </c>
@@ -3572,7 +3569,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A127" s="6" t="s">
         <v>247</v>
       </c>
@@ -3586,7 +3583,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A128" s="6" t="s">
         <v>247</v>
       </c>
@@ -3600,7 +3597,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A129" s="6" t="s">
         <v>247</v>
       </c>
@@ -3614,7 +3611,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A131" s="6" t="s">
         <v>259</v>
       </c>
@@ -3628,7 +3625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A132" s="6" t="s">
         <v>259</v>
       </c>
@@ -3642,7 +3639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A133" s="6" t="s">
         <v>259</v>
       </c>
@@ -3656,7 +3653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A134" s="6" t="s">
         <v>259</v>
       </c>
@@ -3670,7 +3667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A135" s="6" t="s">
         <v>259</v>
       </c>
@@ -3684,7 +3681,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A137" s="6" t="s">
         <v>261</v>
       </c>
@@ -3698,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A138" s="6" t="s">
         <v>261</v>
       </c>
@@ -3712,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A140" s="6" t="s">
         <v>262</v>
       </c>
@@ -3726,7 +3723,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A141" s="6" t="s">
         <v>262</v>
       </c>
@@ -3740,7 +3737,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A142" s="6" t="s">
         <v>262</v>
       </c>
@@ -3754,7 +3751,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A143" s="6" t="s">
         <v>262</v>
       </c>
@@ -3768,7 +3765,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A144" s="6" t="s">
         <v>262</v>
       </c>
@@ -3782,7 +3779,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A146" s="6" t="s">
         <v>263</v>
       </c>
@@ -3796,7 +3793,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A147" s="6" t="s">
         <v>263</v>
       </c>
@@ -3810,7 +3807,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A148" s="6" t="s">
         <v>263</v>
       </c>
@@ -3824,7 +3821,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A149" s="6" t="s">
         <v>263</v>
       </c>
@@ -3838,7 +3835,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A150" s="6" t="s">
         <v>263</v>
       </c>
@@ -3852,7 +3849,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A152" s="6" t="s">
         <v>285</v>
       </c>
@@ -3866,7 +3863,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A153" s="6" t="s">
         <v>285</v>
       </c>
@@ -3880,7 +3877,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A154" s="6" t="s">
         <v>285</v>
       </c>
@@ -3894,7 +3891,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A155" s="6" t="s">
         <v>285</v>
       </c>
@@ -3908,7 +3905,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A157" s="6" t="s">
         <v>289</v>
       </c>
@@ -3922,7 +3919,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A158" s="6" t="s">
         <v>289</v>
       </c>
@@ -3936,7 +3933,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A159" s="6" t="s">
         <v>289</v>
       </c>
@@ -3950,7 +3947,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A161" s="6" t="s">
         <v>290</v>
       </c>
@@ -3964,7 +3961,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A162" s="6" t="s">
         <v>290</v>
       </c>
@@ -3978,7 +3975,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A163" s="6" t="s">
         <v>290</v>
       </c>
@@ -3992,7 +3989,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A164" s="6" t="s">
         <v>290</v>
       </c>
@@ -4006,7 +4003,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A165" s="6" t="s">
         <v>290</v>
       </c>
@@ -4020,7 +4017,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A167" s="6" t="s">
         <v>301</v>
       </c>
@@ -4034,7 +4031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A168" s="6" t="s">
         <v>301</v>
       </c>
@@ -4048,7 +4045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A169" s="6" t="s">
         <v>301</v>
       </c>
@@ -4062,7 +4059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A170" s="6" t="s">
         <v>301</v>
       </c>
@@ -4076,7 +4073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A171" s="6" t="s">
         <v>301</v>
       </c>
@@ -4090,7 +4087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A172" s="6" t="s">
         <v>301</v>
       </c>
@@ -4104,7 +4101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A173" s="6" t="s">
         <v>301</v>
       </c>
@@ -4118,7 +4115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A175" s="6" t="s">
         <v>302</v>
       </c>
@@ -4132,7 +4129,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A176" s="6" t="s">
         <v>302</v>
       </c>
@@ -4146,7 +4143,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A177" s="6" t="s">
         <v>302</v>
       </c>
@@ -4160,7 +4157,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A179" s="6" t="s">
         <v>309</v>
       </c>
@@ -4174,7 +4171,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A180" s="6" t="s">
         <v>309</v>
       </c>
@@ -4188,7 +4185,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A181" s="6" t="s">
         <v>309</v>
       </c>
@@ -4202,7 +4199,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A183" s="6" t="s">
         <v>315</v>
       </c>
@@ -4216,7 +4213,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A184" s="6" t="s">
         <v>315</v>
       </c>
@@ -4230,7 +4227,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A185" s="6" t="s">
         <v>315</v>
       </c>
@@ -4244,7 +4241,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A186" s="6" t="s">
         <v>315</v>
       </c>
@@ -4258,7 +4255,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A187" s="6" t="s">
         <v>315</v>
       </c>
@@ -4272,7 +4269,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A189" s="6" t="s">
         <v>321</v>
       </c>
@@ -4286,7 +4283,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A190" s="6" t="s">
         <v>321</v>
       </c>
@@ -4300,7 +4297,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A191" s="6" t="s">
         <v>321</v>
       </c>
@@ -4314,7 +4311,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A192" s="6" t="s">
         <v>321</v>
       </c>
@@ -4328,7 +4325,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.95">
       <c r="A193" s="6" t="s">
         <v>321</v>
       </c>

</xml_diff>